<commit_message>
Fix error displaying in Report
</commit_message>
<xml_diff>
--- a/PO Summary.xlsx
+++ b/PO Summary.xlsx
@@ -15,7 +15,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" uniqueCount="38">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" uniqueCount="190">
   <si>
     <t>PO Summary 2021</t>
   </si>
@@ -74,61 +74,544 @@
     <t>Remarks</t>
   </si>
   <si>
-    <t>itb21-1000-CNPR</t>
-  </si>
-  <si>
-    <t>smaple purpose</t>
-  </si>
-  <si>
-    <t>sample end use</t>
-  </si>
-  <si>
-    <t>2021-05-05</t>
-  </si>
-  <si>
-    <t>Pitb21-1000-1000-CNPR</t>
-  </si>
-  <si>
-    <t>hen</t>
-  </si>
-  <si>
-    <t>pc/s</t>
-  </si>
-  <si>
-    <t xml:space="preserve">item 1 </t>
-  </si>
-  <si>
-    <t>Pending</t>
-  </si>
-  <si>
-    <t>AOQ Done - For TE - 2021-05-05</t>
-  </si>
-  <si>
-    <t>A. H. C. Rewinding Shop</t>
+    <t>EIC20-1438-CNPR</t>
+  </si>
+  <si>
+    <t>EIC Consumables</t>
+  </si>
+  <si>
+    <t>EIC</t>
+  </si>
+  <si>
+    <t>2020-10-21</t>
+  </si>
+  <si>
+    <t>PEIC20-1438-2026-CNPR</t>
+  </si>
+  <si>
+    <t>Kennah Sasamoto</t>
+  </si>
+  <si>
+    <t>pcs</t>
+  </si>
+  <si>
+    <t>Electrical Tape; Vinyl (Big), brand: Armak</t>
+  </si>
+  <si>
+    <t>Fully Delivered</t>
+  </si>
+  <si>
+    <t xml:space="preserve">10.23.2020 - Delivered DR# 1961-CNPR
+</t>
+  </si>
+  <si>
+    <t>HKL Enterprises Incorporated</t>
   </si>
   <si>
     <t>COD</t>
   </si>
   <si>
-    <t xml:space="preserve"> 150.00</t>
-  </si>
-  <si>
-    <t>Pitb21-1000-1001-CNPR</t>
-  </si>
-  <si>
-    <t>Pitb21-1000-1002-CNPR</t>
-  </si>
-  <si>
-    <t>Pitb21-1000-1007-CNPR</t>
-  </si>
-  <si>
-    <t xml:space="preserve">item 1, </t>
-  </si>
-  <si>
-    <t>A &amp; M Medcare Products Distributors</t>
-  </si>
-  <si>
-    <t>PHP 140.00</t>
+    <t xml:space="preserve"> 28.5000</t>
+  </si>
+  <si>
+    <t>PEIC20-1438-2027-CNPR</t>
+  </si>
+  <si>
+    <t>pairs</t>
+  </si>
+  <si>
+    <t>Gloves; Cotton with rubber, Brand: Ingco</t>
+  </si>
+  <si>
+    <t xml:space="preserve">10.23.2020 - Delivered DR# 1962-CNPR
+</t>
+  </si>
+  <si>
+    <t>A-one Industrial Sales</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> 41.0000</t>
+  </si>
+  <si>
+    <t>PEIC20-1438-2028-CNPR</t>
+  </si>
+  <si>
+    <t>Brush; Steel</t>
+  </si>
+  <si>
+    <t xml:space="preserve">11.19.2020 - Delivered DR# 2046-CNPR
+</t>
+  </si>
+  <si>
+    <t>Greenlane Hardware and Construction Supply Inc</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> 16.0000</t>
+  </si>
+  <si>
+    <t>PEIC20-1438-2029-CNPR</t>
+  </si>
+  <si>
+    <t>pc</t>
+  </si>
+  <si>
+    <t xml:space="preserve">	Brush, Paint, 1"</t>
+  </si>
+  <si>
+    <t xml:space="preserve">10.23.2020 - Delivered DR# 1964-CNPR
+</t>
+  </si>
+  <si>
+    <t>Visayan Construction Supply</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> 15.0000</t>
+  </si>
+  <si>
+    <t>PEIC20-1438-2030-CNPR</t>
+  </si>
+  <si>
+    <t>Battery; AAA, Brand: Energizer</t>
+  </si>
+  <si>
+    <t xml:space="preserve">10.23.2020 - Delivered DR# 1965-CNPR
+</t>
+  </si>
+  <si>
+    <t>New Llacer Electronics &amp; Electrical Supply</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> 55.0000</t>
+  </si>
+  <si>
+    <t>PEIC20-1438-2031-CNPR</t>
+  </si>
+  <si>
+    <t>pcs.</t>
+  </si>
+  <si>
+    <t>Battery; AA, Brand: Energizer</t>
+  </si>
+  <si>
+    <t xml:space="preserve">10.23.2020 - Delivered DR# 1966-CNPR
+</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> 49.0000</t>
+  </si>
+  <si>
+    <t>PEIC20-1438-2032-CNPR</t>
+  </si>
+  <si>
+    <t>gallon</t>
+  </si>
+  <si>
+    <t>Soap; Liquid</t>
+  </si>
+  <si>
+    <t xml:space="preserve">10.23.2020 - Delivered DR# 1967-CNPR
+</t>
+  </si>
+  <si>
+    <t>TMVG Multi-Sales, Inc.</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> 280.0000</t>
+  </si>
+  <si>
+    <t>2020-10-22</t>
+  </si>
+  <si>
+    <t>PEIC20-1438-2033-CNPR</t>
+  </si>
+  <si>
+    <t>Terminal lugs; 14mm2, long barrel, single hole</t>
+  </si>
+  <si>
+    <t xml:space="preserve">10.23.2020 - Delivered DR# 1968-CNPR
+</t>
+  </si>
+  <si>
+    <t>AA Electrical Supply</t>
+  </si>
+  <si>
+    <t>30 days PDC</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> 95.0000</t>
+  </si>
+  <si>
+    <t>Terminal lugs; 32mm2, long barrel, single hole</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> 100.0000</t>
+  </si>
+  <si>
+    <t>Terminal lugs; #16-14 awg, insulated pin type</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> 5.0000</t>
+  </si>
+  <si>
+    <t>Terminal lugs; #12-10 awg, insulated pin type</t>
+  </si>
+  <si>
+    <t xml:space="preserve">10.23.2020 - Delivered DR# 1968-CNPR
+10.25.2020 - Delivered DR# 1975-CNPR
+</t>
+  </si>
+  <si>
+    <t>2020-10-27</t>
+  </si>
+  <si>
+    <t>PEIC20-1438-2053-CNPR</t>
+  </si>
+  <si>
+    <t>kgs.</t>
+  </si>
+  <si>
+    <t>Rags; Cotton</t>
+  </si>
+  <si>
+    <t xml:space="preserve">11.03.2020 - Delivered DR# 1989-CNPR
+</t>
+  </si>
+  <si>
+    <t>Procolors T-Shirts Printing</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> 50.0000</t>
+  </si>
+  <si>
+    <t>2020-10-28</t>
+  </si>
+  <si>
+    <t>PEIC20-1438-2054-CNPR</t>
+  </si>
+  <si>
+    <t>cans</t>
+  </si>
+  <si>
+    <t xml:space="preserve">	Penetrant Multi Use WD-40 Net Content: 333 mL / 311G / 12.9 FL.OZ</t>
+  </si>
+  <si>
+    <t xml:space="preserve">11.07.2020 - Delivered DR# 1990-CNPR
+</t>
+  </si>
+  <si>
+    <t>Ace Hardware Philippines, Inc. - Bacolod Branch</t>
+  </si>
+  <si>
+    <t>Cash, Check Payment subject for clearing</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> 254.7500</t>
+  </si>
+  <si>
+    <t>can</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> Cleaner Contact Specialist Fast Drying WD 40 360 mL</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> 429.7500</t>
+  </si>
+  <si>
+    <t>2020-10-30</t>
+  </si>
+  <si>
+    <t>PEIC20-1438-2068-CNPR</t>
+  </si>
+  <si>
+    <t>Cable tie; 450mm (18") (10pcs/ bundle), Brand: Arrow</t>
+  </si>
+  <si>
+    <t xml:space="preserve">11.13.2020 - Delivered DR# 2002-CNPR
+</t>
+  </si>
+  <si>
+    <t>Jas't Marketing Co.</t>
+  </si>
+  <si>
+    <t>30 days</t>
+  </si>
+  <si>
+    <t>PHP 7.4000</t>
+  </si>
+  <si>
+    <t>Cable tie; 100mm, 4" (100pcs/pack), Brand: Arrow</t>
+  </si>
+  <si>
+    <t>PHP 0.1600</t>
+  </si>
+  <si>
+    <t>Fluorescent; holder, Brand: Kopez</t>
+  </si>
+  <si>
+    <t>PHP 20.0000</t>
+  </si>
+  <si>
+    <t>Starter; switch holder, Brand: Kopez</t>
+  </si>
+  <si>
+    <t>2020-11-10</t>
+  </si>
+  <si>
+    <t>PEIC20-1438-2079-CNPR</t>
+  </si>
+  <si>
+    <t>rolls</t>
+  </si>
+  <si>
+    <t>Masking Tape 1/2", Brand: Armak</t>
+  </si>
+  <si>
+    <t xml:space="preserve">11.19.2020 - Delivered DR# 2013-CNPR
+</t>
+  </si>
+  <si>
+    <t>Masking Tape 1", Brand: Armak</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> 28.0000</t>
+  </si>
+  <si>
+    <t>PEIC20-1438-2080-CNPR</t>
+  </si>
+  <si>
+    <t>gal</t>
+  </si>
+  <si>
+    <t>Alcohol; Denatured</t>
+  </si>
+  <si>
+    <t xml:space="preserve">11.17.2020 - Delivered DR# 2014-CNPR
+</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> 240.0000</t>
+  </si>
+  <si>
+    <t>sheets</t>
+  </si>
+  <si>
+    <t>Paper; Abrasive 180, water resistant, Brand: Creston</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> 12.0000</t>
+  </si>
+  <si>
+    <t>PEIC20-1438-2081-CNPR</t>
+  </si>
+  <si>
+    <t>Pc</t>
+  </si>
+  <si>
+    <t>Drill bit; Masonry, 1/4", Brand: Powerhouse</t>
+  </si>
+  <si>
+    <t xml:space="preserve">11.19.2020 - Delivered DR# 2030-CNPR
+</t>
+  </si>
+  <si>
+    <t>PEIC20-1438-2095-CNPR</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Drill Bit; Metal, 1/8", Brand: Creston </t>
+  </si>
+  <si>
+    <t xml:space="preserve">11.17.2020 - Delivered DR# 2029-CNPR
+</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> 22.0000</t>
+  </si>
+  <si>
+    <t>PEIC20-1438-2096-CNPR</t>
+  </si>
+  <si>
+    <t>Bit; Drill, Steel, 1/4", Brand: Dormer</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> 127.2500</t>
+  </si>
+  <si>
+    <t>2020-11-11</t>
+  </si>
+  <si>
+    <t>PEIC20-1438-2110-CNPR</t>
+  </si>
+  <si>
+    <t>Gloves; Cotton</t>
+  </si>
+  <si>
+    <t xml:space="preserve">11.19.2020 - Delivered DR# 2044-CNPR
+</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> 11.4500</t>
+  </si>
+  <si>
+    <t>PEIC20-1438-2111-CNPR</t>
+  </si>
+  <si>
+    <t>Sugarland Hardware Corp.</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> 18.0000</t>
+  </si>
+  <si>
+    <t>PEIC20-1438-2113-CNPR</t>
+  </si>
+  <si>
+    <t>Battery; Rechargeable  AA, 1500 mAH, Brand: Eneloop</t>
+  </si>
+  <si>
+    <t xml:space="preserve">11.19.2020 - Delivered DR# 2047-CNPR
+</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> 207.5000</t>
+  </si>
+  <si>
+    <t>2020-11-17</t>
+  </si>
+  <si>
+    <t>PEIC20-1438-2137-CNPR</t>
+  </si>
+  <si>
+    <t>Blade; Hacksaw, HSS, 300mm/12" , 18TPI, Brand: Lenox</t>
+  </si>
+  <si>
+    <t xml:space="preserve">11.25.2020 - Delivered DR# 2069-CNPR
+</t>
+  </si>
+  <si>
+    <t>SGS Hardware Corporation</t>
+  </si>
+  <si>
+    <t>PEIC20-1438-2138-CNPR</t>
+  </si>
+  <si>
+    <t>Broom; Buri (Damul)</t>
+  </si>
+  <si>
+    <t xml:space="preserve">11.25.2020 - Delivered DR# 2070-CNPR
+</t>
+  </si>
+  <si>
+    <t>Native Store</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> 70.0000</t>
+  </si>
+  <si>
+    <t>PEIC20-1438-2139-CNPR</t>
+  </si>
+  <si>
+    <t>quarts</t>
+  </si>
+  <si>
+    <t>Water, Distilled</t>
+  </si>
+  <si>
+    <t xml:space="preserve">11.27.2020 - Delivered DR# 2071-CNPR
+</t>
+  </si>
+  <si>
+    <t>Samson Merchandising Inc.</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> 10.0000</t>
+  </si>
+  <si>
+    <t>PEIC20-1438-2140-CNPR</t>
+  </si>
+  <si>
+    <t>pack</t>
+  </si>
+  <si>
+    <t>Tie Cable, 150mm x 4mm</t>
+  </si>
+  <si>
+    <t xml:space="preserve">11.27.2020 - Delivered DR# 2072-CNPR (1.00 pack)
+</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> 45.0000</t>
+  </si>
+  <si>
+    <t>PEIC20-1438-2141-CNPR</t>
+  </si>
+  <si>
+    <t>piece</t>
+  </si>
+  <si>
+    <t>Battery; 1.5Volts, C Size, Brand: Eveready (Black)</t>
+  </si>
+  <si>
+    <t xml:space="preserve">11.27.2020 - Delivered DR# 2073-CNPR
+</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> 31.0000</t>
+  </si>
+  <si>
+    <t>2021-02-01</t>
+  </si>
+  <si>
+    <t>PEIC20-1438-2149-CNPR</t>
+  </si>
+  <si>
+    <t>Terminal lugs; 8mm2, long barrel, single hole</t>
+  </si>
+  <si>
+    <t xml:space="preserve">02.05.2021 - Delivered DR# 2366-CNPR
+</t>
+  </si>
+  <si>
+    <t>PHP 75.0000</t>
+  </si>
+  <si>
+    <t>Terminal lugs; 80mm2, long barrel, single hole</t>
+  </si>
+  <si>
+    <t>PHP 180.0000</t>
+  </si>
+  <si>
+    <t>2020-11-26</t>
+  </si>
+  <si>
+    <t>PEIC20-1438-2150-CNPR</t>
+  </si>
+  <si>
+    <t>length</t>
+  </si>
+  <si>
+    <t>Din; Rail, 1 length = 1 meter</t>
+  </si>
+  <si>
+    <t xml:space="preserve">12.03.2020 - Delivered DR# 2088-CNPR (1.00 length)
+</t>
+  </si>
+  <si>
+    <t>PHP 72.0000</t>
+  </si>
+  <si>
+    <t>2020-12-15</t>
+  </si>
+  <si>
+    <t>PEIC20-1438-2239-CNPR</t>
+  </si>
+  <si>
+    <t>Masking; tape 1/4", Brand: Nikon</t>
+  </si>
+  <si>
+    <t xml:space="preserve">12.16.2020 - Delivered DR# 2165-CNPR
+</t>
+  </si>
+  <si>
+    <t>Bacolod Paint Marketing</t>
   </si>
 </sst>
 </file>
@@ -165,13 +648,19 @@
       <name val="Arial Black"/>
     </font>
   </fonts>
-  <fills count="2">
+  <fills count="3">
     <fill>
       <patternFill patternType="none"/>
     </fill>
     <fill>
       <patternFill patternType="gray125">
         <fgColor rgb="FFFFFFFF"/>
+        <bgColor rgb="FF000000"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFbcffc7"/>
         <bgColor rgb="FF000000"/>
       </patternFill>
     </fill>
@@ -196,7 +685,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="7">
+  <cellXfs count="8">
     <xf xfId="0" fontId="0" numFmtId="0" fillId="0" borderId="0" applyFont="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" shrinkToFit="false"/>
     </xf>
@@ -209,14 +698,17 @@
     <xf xfId="0" fontId="1" numFmtId="0" fillId="0" borderId="1" applyFont="1" applyNumberFormat="0" applyFill="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="false" shrinkToFit="false"/>
     </xf>
-    <xf xfId="0" fontId="0" numFmtId="0" fillId="0" borderId="1" applyFont="0" applyNumberFormat="0" applyFill="0" applyBorder="1" applyAlignment="1">
+    <xf xfId="0" fontId="0" numFmtId="0" fillId="2" borderId="1" applyFont="0" applyNumberFormat="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="false" shrinkToFit="false"/>
     </xf>
-    <xf xfId="0" fontId="0" numFmtId="0" fillId="0" borderId="1" applyFont="0" applyNumberFormat="0" applyFill="0" applyBorder="1" applyAlignment="0">
+    <xf xfId="0" fontId="0" numFmtId="0" fillId="2" borderId="1" applyFont="0" applyNumberFormat="0" applyFill="1" applyBorder="1" applyAlignment="0">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" shrinkToFit="false"/>
     </xf>
-    <xf xfId="0" fontId="0" numFmtId="4" fillId="0" borderId="1" applyFont="0" applyNumberFormat="1" applyFill="0" applyBorder="1" applyAlignment="1">
+    <xf xfId="0" fontId="0" numFmtId="4" fillId="2" borderId="1" applyFont="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="false" shrinkToFit="false"/>
+    </xf>
+    <xf xfId="0" fontId="0" numFmtId="0" fillId="2" borderId="1" applyFont="0" applyNumberFormat="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="true" shrinkToFit="false"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -517,29 +1009,29 @@
   <sheetPr>
     <outlinePr summaryBelow="1" summaryRight="1"/>
   </sheetPr>
-  <dimension ref="A1:Q8"/>
+  <dimension ref="A1:Q41"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0" showGridLines="true" showRowColHeaders="1">
-      <selection activeCell="Q8" sqref="Q8"/>
+      <selection activeCell="K41" sqref="K41"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
     <col min="1" max="1" width="25.279541" bestFit="true" customWidth="true" style="0"/>
-    <col min="2" max="2" width="17.567139" bestFit="true" customWidth="true" style="0"/>
-    <col min="3" max="3" width="17.567139" bestFit="true" customWidth="true" style="0"/>
+    <col min="2" max="2" width="18.709717" bestFit="true" customWidth="true" style="0"/>
+    <col min="3" max="3" width="8.140869" bestFit="true" customWidth="true" style="0"/>
     <col min="4" max="4" width="12.854004" bestFit="true" customWidth="true" style="0"/>
     <col min="5" max="5" width="25.85083" bestFit="true" customWidth="true" style="0"/>
-    <col min="6" max="6" width="15.281982" bestFit="true" customWidth="true" style="0"/>
+    <col min="6" max="6" width="18.709717" bestFit="true" customWidth="true" style="0"/>
     <col min="7" max="7" width="8.140869" bestFit="true" customWidth="true" style="0"/>
     <col min="8" max="8" width="15.281982" bestFit="true" customWidth="true" style="0"/>
-    <col min="9" max="9" width="5.855713" bestFit="true" customWidth="true" style="0"/>
-    <col min="10" max="10" width="19.995117" bestFit="true" customWidth="true" style="0"/>
-    <col min="11" max="11" width="9.283447" bestFit="true" customWidth="true" style="0"/>
-    <col min="12" max="12" width="36.419678" bestFit="true" customWidth="true" style="0"/>
-    <col min="13" max="13" width="42.418213" bestFit="true" customWidth="true" style="0"/>
-    <col min="14" max="14" width="16.424561" bestFit="true" customWidth="true" style="0"/>
-    <col min="15" max="15" width="12.854004" bestFit="true" customWidth="true" style="0"/>
+    <col min="9" max="9" width="8.140869" bestFit="true" customWidth="true" style="0"/>
+    <col min="10" max="10" width="78.980713" bestFit="true" customWidth="true" style="0"/>
+    <col min="11" max="11" width="18.709717" bestFit="true" customWidth="true" style="0"/>
+    <col min="12" max="12" width="60.128174" bestFit="true" customWidth="true" style="0"/>
+    <col min="13" max="13" width="56.557617" bestFit="true" customWidth="true" style="0"/>
+    <col min="14" max="14" width="48.273926" bestFit="true" customWidth="true" style="0"/>
+    <col min="15" max="15" width="15.281982" bestFit="true" customWidth="true" style="0"/>
     <col min="16" max="16" width="13.996582" bestFit="true" customWidth="true" style="0"/>
     <col min="17" max="17" width="9.283447" bestFit="true" customWidth="true" style="0"/>
   </cols>
@@ -634,7 +1126,7 @@
         <v>5</v>
       </c>
       <c r="H5" s="4">
-        <v>0</v>
+        <v>5</v>
       </c>
       <c r="I5" s="4" t="s">
         <v>25</v>
@@ -642,7 +1134,7 @@
       <c r="J5" s="5" t="s">
         <v>26</v>
       </c>
-      <c r="K5" s="5" t="s">
+      <c r="K5" s="7" t="s">
         <v>27</v>
       </c>
       <c r="L5" s="5" t="s">
@@ -658,7 +1150,7 @@
         <v>31</v>
       </c>
       <c r="P5" s="6">
-        <v>0</v>
+        <v>142.5</v>
       </c>
       <c r="Q5" s="5"/>
     </row>
@@ -682,34 +1174,32 @@
         <v>24</v>
       </c>
       <c r="G6" s="4">
-        <v>5</v>
+        <v>10</v>
       </c>
       <c r="H6" s="4">
-        <v>0</v>
+        <v>10</v>
       </c>
       <c r="I6" s="4" t="s">
-        <v>25</v>
+        <v>33</v>
       </c>
       <c r="J6" s="5" t="s">
-        <v>26</v>
-      </c>
-      <c r="K6" s="5" t="s">
+        <v>34</v>
+      </c>
+      <c r="K6" s="7" t="s">
         <v>27</v>
       </c>
       <c r="L6" s="5" t="s">
-        <v>28</v>
+        <v>35</v>
       </c>
       <c r="M6" s="5" t="s">
-        <v>29</v>
-      </c>
-      <c r="N6" s="5" t="s">
-        <v>30</v>
-      </c>
+        <v>36</v>
+      </c>
+      <c r="N6" s="5"/>
       <c r="O6" s="6" t="s">
-        <v>31</v>
+        <v>37</v>
       </c>
       <c r="P6" s="6">
-        <v>0</v>
+        <v>410</v>
       </c>
       <c r="Q6" s="5"/>
     </row>
@@ -727,13 +1217,13 @@
         <v>22</v>
       </c>
       <c r="E7" s="5" t="s">
-        <v>33</v>
+        <v>38</v>
       </c>
       <c r="F7" s="5" t="s">
         <v>24</v>
       </c>
       <c r="G7" s="4">
-        <v>2</v>
+        <v>3</v>
       </c>
       <c r="H7" s="4">
         <v>0</v>
@@ -742,22 +1232,22 @@
         <v>25</v>
       </c>
       <c r="J7" s="5" t="s">
-        <v>26</v>
-      </c>
-      <c r="K7" s="5" t="s">
+        <v>39</v>
+      </c>
+      <c r="K7" s="7" t="s">
         <v>27</v>
       </c>
       <c r="L7" s="5" t="s">
-        <v>28</v>
+        <v>40</v>
       </c>
       <c r="M7" s="5" t="s">
-        <v>29</v>
+        <v>41</v>
       </c>
       <c r="N7" s="5" t="s">
         <v>30</v>
       </c>
       <c r="O7" s="6" t="s">
-        <v>31</v>
+        <v>42</v>
       </c>
       <c r="P7" s="6">
         <v>0</v>
@@ -778,42 +1268,1723 @@
         <v>22</v>
       </c>
       <c r="E8" s="5" t="s">
-        <v>34</v>
+        <v>43</v>
       </c>
       <c r="F8" s="5" t="s">
         <v>24</v>
       </c>
       <c r="G8" s="4">
-        <v>5</v>
+        <v>3</v>
       </c>
       <c r="H8" s="4">
-        <v>0</v>
+        <v>3</v>
       </c>
       <c r="I8" s="4" t="s">
-        <v>25</v>
+        <v>44</v>
       </c>
       <c r="J8" s="5" t="s">
-        <v>35</v>
-      </c>
-      <c r="K8" s="5" t="s">
+        <v>45</v>
+      </c>
+      <c r="K8" s="7" t="s">
         <v>27</v>
       </c>
       <c r="L8" s="5" t="s">
-        <v>28</v>
+        <v>46</v>
       </c>
       <c r="M8" s="5" t="s">
-        <v>36</v>
+        <v>47</v>
       </c>
       <c r="N8" s="5" t="s">
         <v>30</v>
       </c>
       <c r="O8" s="6" t="s">
+        <v>48</v>
+      </c>
+      <c r="P8" s="6">
+        <v>45</v>
+      </c>
+      <c r="Q8" s="5"/>
+    </row>
+    <row r="9" spans="1:17">
+      <c r="A9" s="4" t="s">
+        <v>19</v>
+      </c>
+      <c r="B9" s="5" t="s">
+        <v>20</v>
+      </c>
+      <c r="C9" s="5" t="s">
+        <v>21</v>
+      </c>
+      <c r="D9" s="5" t="s">
+        <v>22</v>
+      </c>
+      <c r="E9" s="5" t="s">
+        <v>49</v>
+      </c>
+      <c r="F9" s="5" t="s">
+        <v>24</v>
+      </c>
+      <c r="G9" s="4">
+        <v>4</v>
+      </c>
+      <c r="H9" s="4">
+        <v>4</v>
+      </c>
+      <c r="I9" s="4" t="s">
+        <v>25</v>
+      </c>
+      <c r="J9" s="5" t="s">
+        <v>50</v>
+      </c>
+      <c r="K9" s="7" t="s">
+        <v>27</v>
+      </c>
+      <c r="L9" s="5" t="s">
+        <v>51</v>
+      </c>
+      <c r="M9" s="5" t="s">
+        <v>52</v>
+      </c>
+      <c r="N9" s="5" t="s">
+        <v>30</v>
+      </c>
+      <c r="O9" s="6" t="s">
+        <v>53</v>
+      </c>
+      <c r="P9" s="6">
+        <v>220</v>
+      </c>
+      <c r="Q9" s="5"/>
+    </row>
+    <row r="10" spans="1:17">
+      <c r="A10" s="4" t="s">
+        <v>19</v>
+      </c>
+      <c r="B10" s="5" t="s">
+        <v>20</v>
+      </c>
+      <c r="C10" s="5" t="s">
+        <v>21</v>
+      </c>
+      <c r="D10" s="5" t="s">
+        <v>22</v>
+      </c>
+      <c r="E10" s="5" t="s">
+        <v>54</v>
+      </c>
+      <c r="F10" s="5" t="s">
+        <v>24</v>
+      </c>
+      <c r="G10" s="4">
+        <v>6</v>
+      </c>
+      <c r="H10" s="4">
+        <v>6</v>
+      </c>
+      <c r="I10" s="4" t="s">
+        <v>55</v>
+      </c>
+      <c r="J10" s="5" t="s">
+        <v>56</v>
+      </c>
+      <c r="K10" s="7" t="s">
+        <v>27</v>
+      </c>
+      <c r="L10" s="5" t="s">
+        <v>57</v>
+      </c>
+      <c r="M10" s="5" t="s">
+        <v>52</v>
+      </c>
+      <c r="N10" s="5" t="s">
+        <v>30</v>
+      </c>
+      <c r="O10" s="6" t="s">
+        <v>58</v>
+      </c>
+      <c r="P10" s="6">
+        <v>294</v>
+      </c>
+      <c r="Q10" s="5"/>
+    </row>
+    <row r="11" spans="1:17">
+      <c r="A11" s="4" t="s">
+        <v>19</v>
+      </c>
+      <c r="B11" s="5" t="s">
+        <v>20</v>
+      </c>
+      <c r="C11" s="5" t="s">
+        <v>21</v>
+      </c>
+      <c r="D11" s="5" t="s">
+        <v>22</v>
+      </c>
+      <c r="E11" s="5" t="s">
+        <v>59</v>
+      </c>
+      <c r="F11" s="5" t="s">
+        <v>24</v>
+      </c>
+      <c r="G11" s="4">
+        <v>1</v>
+      </c>
+      <c r="H11" s="4">
+        <v>1</v>
+      </c>
+      <c r="I11" s="4" t="s">
+        <v>60</v>
+      </c>
+      <c r="J11" s="5" t="s">
+        <v>61</v>
+      </c>
+      <c r="K11" s="7" t="s">
+        <v>27</v>
+      </c>
+      <c r="L11" s="5" t="s">
+        <v>62</v>
+      </c>
+      <c r="M11" s="5" t="s">
+        <v>63</v>
+      </c>
+      <c r="N11" s="5" t="s">
+        <v>30</v>
+      </c>
+      <c r="O11" s="6" t="s">
+        <v>64</v>
+      </c>
+      <c r="P11" s="6">
+        <v>280</v>
+      </c>
+      <c r="Q11" s="5"/>
+    </row>
+    <row r="12" spans="1:17">
+      <c r="A12" s="4" t="s">
+        <v>19</v>
+      </c>
+      <c r="B12" s="5" t="s">
+        <v>20</v>
+      </c>
+      <c r="C12" s="5" t="s">
+        <v>21</v>
+      </c>
+      <c r="D12" s="5" t="s">
+        <v>65</v>
+      </c>
+      <c r="E12" s="5" t="s">
+        <v>66</v>
+      </c>
+      <c r="F12" s="5" t="s">
+        <v>24</v>
+      </c>
+      <c r="G12" s="4">
+        <v>20</v>
+      </c>
+      <c r="H12" s="4">
+        <v>20</v>
+      </c>
+      <c r="I12" s="4" t="s">
+        <v>55</v>
+      </c>
+      <c r="J12" s="5" t="s">
+        <v>67</v>
+      </c>
+      <c r="K12" s="7" t="s">
+        <v>27</v>
+      </c>
+      <c r="L12" s="5" t="s">
+        <v>68</v>
+      </c>
+      <c r="M12" s="5" t="s">
+        <v>69</v>
+      </c>
+      <c r="N12" s="5" t="s">
+        <v>70</v>
+      </c>
+      <c r="O12" s="6" t="s">
+        <v>71</v>
+      </c>
+      <c r="P12" s="6">
+        <v>1900</v>
+      </c>
+      <c r="Q12" s="5"/>
+    </row>
+    <row r="13" spans="1:17">
+      <c r="A13" s="4" t="s">
+        <v>19</v>
+      </c>
+      <c r="B13" s="5" t="s">
+        <v>20</v>
+      </c>
+      <c r="C13" s="5" t="s">
+        <v>21</v>
+      </c>
+      <c r="D13" s="5" t="s">
+        <v>65</v>
+      </c>
+      <c r="E13" s="5" t="s">
+        <v>66</v>
+      </c>
+      <c r="F13" s="5" t="s">
+        <v>24</v>
+      </c>
+      <c r="G13" s="4">
+        <v>20</v>
+      </c>
+      <c r="H13" s="4">
+        <v>20</v>
+      </c>
+      <c r="I13" s="4" t="s">
+        <v>55</v>
+      </c>
+      <c r="J13" s="5" t="s">
+        <v>72</v>
+      </c>
+      <c r="K13" s="7" t="s">
+        <v>27</v>
+      </c>
+      <c r="L13" s="5" t="s">
+        <v>68</v>
+      </c>
+      <c r="M13" s="5" t="s">
+        <v>69</v>
+      </c>
+      <c r="N13" s="5" t="s">
+        <v>70</v>
+      </c>
+      <c r="O13" s="6" t="s">
+        <v>73</v>
+      </c>
+      <c r="P13" s="6">
+        <v>2000</v>
+      </c>
+      <c r="Q13" s="5"/>
+    </row>
+    <row r="14" spans="1:17">
+      <c r="A14" s="4" t="s">
+        <v>19</v>
+      </c>
+      <c r="B14" s="5" t="s">
+        <v>20</v>
+      </c>
+      <c r="C14" s="5" t="s">
+        <v>21</v>
+      </c>
+      <c r="D14" s="5" t="s">
+        <v>65</v>
+      </c>
+      <c r="E14" s="5" t="s">
+        <v>66</v>
+      </c>
+      <c r="F14" s="5" t="s">
+        <v>24</v>
+      </c>
+      <c r="G14" s="4">
+        <v>50</v>
+      </c>
+      <c r="H14" s="4">
+        <v>50</v>
+      </c>
+      <c r="I14" s="4" t="s">
+        <v>55</v>
+      </c>
+      <c r="J14" s="5" t="s">
+        <v>74</v>
+      </c>
+      <c r="K14" s="7" t="s">
+        <v>27</v>
+      </c>
+      <c r="L14" s="5" t="s">
+        <v>68</v>
+      </c>
+      <c r="M14" s="5" t="s">
+        <v>69</v>
+      </c>
+      <c r="N14" s="5" t="s">
+        <v>70</v>
+      </c>
+      <c r="O14" s="6" t="s">
+        <v>75</v>
+      </c>
+      <c r="P14" s="6">
+        <v>250</v>
+      </c>
+      <c r="Q14" s="5"/>
+    </row>
+    <row r="15" spans="1:17">
+      <c r="A15" s="4" t="s">
+        <v>19</v>
+      </c>
+      <c r="B15" s="5" t="s">
+        <v>20</v>
+      </c>
+      <c r="C15" s="5" t="s">
+        <v>21</v>
+      </c>
+      <c r="D15" s="5" t="s">
+        <v>65</v>
+      </c>
+      <c r="E15" s="5" t="s">
+        <v>66</v>
+      </c>
+      <c r="F15" s="5" t="s">
+        <v>24</v>
+      </c>
+      <c r="G15" s="4">
+        <v>50</v>
+      </c>
+      <c r="H15" s="4">
+        <v>50</v>
+      </c>
+      <c r="I15" s="4" t="s">
+        <v>55</v>
+      </c>
+      <c r="J15" s="5" t="s">
+        <v>76</v>
+      </c>
+      <c r="K15" s="7" t="s">
+        <v>27</v>
+      </c>
+      <c r="L15" s="5" t="s">
+        <v>77</v>
+      </c>
+      <c r="M15" s="5" t="s">
+        <v>69</v>
+      </c>
+      <c r="N15" s="5" t="s">
+        <v>70</v>
+      </c>
+      <c r="O15" s="6" t="s">
+        <v>75</v>
+      </c>
+      <c r="P15" s="6">
+        <v>250</v>
+      </c>
+      <c r="Q15" s="5"/>
+    </row>
+    <row r="16" spans="1:17">
+      <c r="A16" s="4" t="s">
+        <v>19</v>
+      </c>
+      <c r="B16" s="5" t="s">
+        <v>20</v>
+      </c>
+      <c r="C16" s="5" t="s">
+        <v>21</v>
+      </c>
+      <c r="D16" s="5" t="s">
+        <v>78</v>
+      </c>
+      <c r="E16" s="5" t="s">
+        <v>79</v>
+      </c>
+      <c r="F16" s="5" t="s">
+        <v>24</v>
+      </c>
+      <c r="G16" s="4">
+        <v>5</v>
+      </c>
+      <c r="H16" s="4">
+        <v>5</v>
+      </c>
+      <c r="I16" s="4" t="s">
+        <v>80</v>
+      </c>
+      <c r="J16" s="5" t="s">
+        <v>81</v>
+      </c>
+      <c r="K16" s="7" t="s">
+        <v>27</v>
+      </c>
+      <c r="L16" s="5" t="s">
+        <v>82</v>
+      </c>
+      <c r="M16" s="5" t="s">
+        <v>83</v>
+      </c>
+      <c r="N16" s="5" t="s">
+        <v>30</v>
+      </c>
+      <c r="O16" s="6" t="s">
+        <v>84</v>
+      </c>
+      <c r="P16" s="6">
+        <v>250</v>
+      </c>
+      <c r="Q16" s="5"/>
+    </row>
+    <row r="17" spans="1:17">
+      <c r="A17" s="4" t="s">
+        <v>19</v>
+      </c>
+      <c r="B17" s="5" t="s">
+        <v>20</v>
+      </c>
+      <c r="C17" s="5" t="s">
+        <v>21</v>
+      </c>
+      <c r="D17" s="5" t="s">
+        <v>85</v>
+      </c>
+      <c r="E17" s="5" t="s">
+        <v>86</v>
+      </c>
+      <c r="F17" s="5" t="s">
+        <v>24</v>
+      </c>
+      <c r="G17" s="4">
+        <v>1</v>
+      </c>
+      <c r="H17" s="4">
+        <v>1</v>
+      </c>
+      <c r="I17" s="4" t="s">
+        <v>87</v>
+      </c>
+      <c r="J17" s="5" t="s">
+        <v>88</v>
+      </c>
+      <c r="K17" s="7" t="s">
+        <v>27</v>
+      </c>
+      <c r="L17" s="5" t="s">
+        <v>89</v>
+      </c>
+      <c r="M17" s="5" t="s">
+        <v>90</v>
+      </c>
+      <c r="N17" s="5" t="s">
+        <v>91</v>
+      </c>
+      <c r="O17" s="6" t="s">
+        <v>92</v>
+      </c>
+      <c r="P17" s="6">
+        <v>254.75</v>
+      </c>
+      <c r="Q17" s="5"/>
+    </row>
+    <row r="18" spans="1:17">
+      <c r="A18" s="4" t="s">
+        <v>19</v>
+      </c>
+      <c r="B18" s="5" t="s">
+        <v>20</v>
+      </c>
+      <c r="C18" s="5" t="s">
+        <v>21</v>
+      </c>
+      <c r="D18" s="5" t="s">
+        <v>85</v>
+      </c>
+      <c r="E18" s="5" t="s">
+        <v>86</v>
+      </c>
+      <c r="F18" s="5" t="s">
+        <v>24</v>
+      </c>
+      <c r="G18" s="4">
+        <v>2</v>
+      </c>
+      <c r="H18" s="4">
+        <v>2</v>
+      </c>
+      <c r="I18" s="4" t="s">
+        <v>93</v>
+      </c>
+      <c r="J18" s="5" t="s">
+        <v>94</v>
+      </c>
+      <c r="K18" s="7" t="s">
+        <v>27</v>
+      </c>
+      <c r="L18" s="5" t="s">
+        <v>89</v>
+      </c>
+      <c r="M18" s="5" t="s">
+        <v>90</v>
+      </c>
+      <c r="N18" s="5" t="s">
+        <v>91</v>
+      </c>
+      <c r="O18" s="6" t="s">
+        <v>95</v>
+      </c>
+      <c r="P18" s="6">
+        <v>859.5</v>
+      </c>
+      <c r="Q18" s="5"/>
+    </row>
+    <row r="19" spans="1:17">
+      <c r="A19" s="4" t="s">
+        <v>19</v>
+      </c>
+      <c r="B19" s="5" t="s">
+        <v>20</v>
+      </c>
+      <c r="C19" s="5" t="s">
+        <v>21</v>
+      </c>
+      <c r="D19" s="5" t="s">
+        <v>96</v>
+      </c>
+      <c r="E19" s="5" t="s">
+        <v>97</v>
+      </c>
+      <c r="F19" s="5" t="s">
+        <v>24</v>
+      </c>
+      <c r="G19" s="4">
+        <v>50</v>
+      </c>
+      <c r="H19" s="4">
+        <v>50</v>
+      </c>
+      <c r="I19" s="4" t="s">
+        <v>55</v>
+      </c>
+      <c r="J19" s="5" t="s">
+        <v>98</v>
+      </c>
+      <c r="K19" s="7" t="s">
+        <v>27</v>
+      </c>
+      <c r="L19" s="5" t="s">
+        <v>99</v>
+      </c>
+      <c r="M19" s="5" t="s">
+        <v>100</v>
+      </c>
+      <c r="N19" s="5" t="s">
+        <v>101</v>
+      </c>
+      <c r="O19" s="6" t="s">
+        <v>102</v>
+      </c>
+      <c r="P19" s="6">
+        <v>370</v>
+      </c>
+      <c r="Q19" s="5"/>
+    </row>
+    <row r="20" spans="1:17">
+      <c r="A20" s="4" t="s">
+        <v>19</v>
+      </c>
+      <c r="B20" s="5" t="s">
+        <v>20</v>
+      </c>
+      <c r="C20" s="5" t="s">
+        <v>21</v>
+      </c>
+      <c r="D20" s="5" t="s">
+        <v>96</v>
+      </c>
+      <c r="E20" s="5" t="s">
+        <v>97</v>
+      </c>
+      <c r="F20" s="5" t="s">
+        <v>24</v>
+      </c>
+      <c r="G20" s="4">
+        <v>100</v>
+      </c>
+      <c r="H20" s="4">
+        <v>100</v>
+      </c>
+      <c r="I20" s="4" t="s">
+        <v>55</v>
+      </c>
+      <c r="J20" s="5" t="s">
+        <v>103</v>
+      </c>
+      <c r="K20" s="7" t="s">
+        <v>27</v>
+      </c>
+      <c r="L20" s="5" t="s">
+        <v>99</v>
+      </c>
+      <c r="M20" s="5" t="s">
+        <v>100</v>
+      </c>
+      <c r="N20" s="5" t="s">
+        <v>101</v>
+      </c>
+      <c r="O20" s="6" t="s">
+        <v>104</v>
+      </c>
+      <c r="P20" s="6">
+        <v>16</v>
+      </c>
+      <c r="Q20" s="5"/>
+    </row>
+    <row r="21" spans="1:17">
+      <c r="A21" s="4" t="s">
+        <v>19</v>
+      </c>
+      <c r="B21" s="5" t="s">
+        <v>20</v>
+      </c>
+      <c r="C21" s="5" t="s">
+        <v>21</v>
+      </c>
+      <c r="D21" s="5" t="s">
+        <v>96</v>
+      </c>
+      <c r="E21" s="5" t="s">
+        <v>97</v>
+      </c>
+      <c r="F21" s="5" t="s">
+        <v>24</v>
+      </c>
+      <c r="G21" s="4">
+        <v>30</v>
+      </c>
+      <c r="H21" s="4">
+        <v>30</v>
+      </c>
+      <c r="I21" s="4" t="s">
+        <v>55</v>
+      </c>
+      <c r="J21" s="5" t="s">
+        <v>105</v>
+      </c>
+      <c r="K21" s="7" t="s">
+        <v>27</v>
+      </c>
+      <c r="L21" s="5" t="s">
+        <v>99</v>
+      </c>
+      <c r="M21" s="5" t="s">
+        <v>100</v>
+      </c>
+      <c r="N21" s="5" t="s">
+        <v>101</v>
+      </c>
+      <c r="O21" s="6" t="s">
+        <v>106</v>
+      </c>
+      <c r="P21" s="6">
+        <v>600</v>
+      </c>
+      <c r="Q21" s="5"/>
+    </row>
+    <row r="22" spans="1:17">
+      <c r="A22" s="4" t="s">
+        <v>19</v>
+      </c>
+      <c r="B22" s="5" t="s">
+        <v>20</v>
+      </c>
+      <c r="C22" s="5" t="s">
+        <v>21</v>
+      </c>
+      <c r="D22" s="5" t="s">
+        <v>96</v>
+      </c>
+      <c r="E22" s="5" t="s">
+        <v>97</v>
+      </c>
+      <c r="F22" s="5" t="s">
+        <v>24</v>
+      </c>
+      <c r="G22" s="4">
+        <v>15</v>
+      </c>
+      <c r="H22" s="4">
+        <v>15</v>
+      </c>
+      <c r="I22" s="4" t="s">
+        <v>55</v>
+      </c>
+      <c r="J22" s="5" t="s">
+        <v>107</v>
+      </c>
+      <c r="K22" s="7" t="s">
+        <v>27</v>
+      </c>
+      <c r="L22" s="5" t="s">
+        <v>99</v>
+      </c>
+      <c r="M22" s="5" t="s">
+        <v>100</v>
+      </c>
+      <c r="N22" s="5" t="s">
+        <v>101</v>
+      </c>
+      <c r="O22" s="6" t="s">
+        <v>106</v>
+      </c>
+      <c r="P22" s="6">
+        <v>300</v>
+      </c>
+      <c r="Q22" s="5"/>
+    </row>
+    <row r="23" spans="1:17">
+      <c r="A23" s="4" t="s">
+        <v>19</v>
+      </c>
+      <c r="B23" s="5" t="s">
+        <v>20</v>
+      </c>
+      <c r="C23" s="5" t="s">
+        <v>21</v>
+      </c>
+      <c r="D23" s="5" t="s">
+        <v>108</v>
+      </c>
+      <c r="E23" s="5" t="s">
+        <v>109</v>
+      </c>
+      <c r="F23" s="5" t="s">
+        <v>24</v>
+      </c>
+      <c r="G23" s="4">
+        <v>2</v>
+      </c>
+      <c r="H23" s="4">
+        <v>2</v>
+      </c>
+      <c r="I23" s="4" t="s">
+        <v>110</v>
+      </c>
+      <c r="J23" s="5" t="s">
+        <v>111</v>
+      </c>
+      <c r="K23" s="7" t="s">
+        <v>27</v>
+      </c>
+      <c r="L23" s="5" t="s">
+        <v>112</v>
+      </c>
+      <c r="M23" s="5" t="s">
+        <v>29</v>
+      </c>
+      <c r="N23" s="5" t="s">
+        <v>30</v>
+      </c>
+      <c r="O23" s="6" t="s">
+        <v>48</v>
+      </c>
+      <c r="P23" s="6">
+        <v>30</v>
+      </c>
+      <c r="Q23" s="5"/>
+    </row>
+    <row r="24" spans="1:17">
+      <c r="A24" s="4" t="s">
+        <v>19</v>
+      </c>
+      <c r="B24" s="5" t="s">
+        <v>20</v>
+      </c>
+      <c r="C24" s="5" t="s">
+        <v>21</v>
+      </c>
+      <c r="D24" s="5" t="s">
+        <v>108</v>
+      </c>
+      <c r="E24" s="5" t="s">
+        <v>109</v>
+      </c>
+      <c r="F24" s="5" t="s">
+        <v>24</v>
+      </c>
+      <c r="G24" s="4">
+        <v>2</v>
+      </c>
+      <c r="H24" s="4">
+        <v>2</v>
+      </c>
+      <c r="I24" s="4" t="s">
+        <v>110</v>
+      </c>
+      <c r="J24" s="5" t="s">
+        <v>113</v>
+      </c>
+      <c r="K24" s="7" t="s">
+        <v>27</v>
+      </c>
+      <c r="L24" s="5" t="s">
+        <v>112</v>
+      </c>
+      <c r="M24" s="5" t="s">
+        <v>29</v>
+      </c>
+      <c r="N24" s="5" t="s">
+        <v>30</v>
+      </c>
+      <c r="O24" s="6" t="s">
+        <v>114</v>
+      </c>
+      <c r="P24" s="6">
+        <v>56</v>
+      </c>
+      <c r="Q24" s="5"/>
+    </row>
+    <row r="25" spans="1:17">
+      <c r="A25" s="4" t="s">
+        <v>19</v>
+      </c>
+      <c r="B25" s="5" t="s">
+        <v>20</v>
+      </c>
+      <c r="C25" s="5" t="s">
+        <v>21</v>
+      </c>
+      <c r="D25" s="5" t="s">
+        <v>108</v>
+      </c>
+      <c r="E25" s="5" t="s">
+        <v>115</v>
+      </c>
+      <c r="F25" s="5" t="s">
+        <v>24</v>
+      </c>
+      <c r="G25" s="4">
+        <v>1</v>
+      </c>
+      <c r="H25" s="4">
+        <v>1</v>
+      </c>
+      <c r="I25" s="4" t="s">
+        <v>116</v>
+      </c>
+      <c r="J25" s="5" t="s">
+        <v>117</v>
+      </c>
+      <c r="K25" s="7" t="s">
+        <v>27</v>
+      </c>
+      <c r="L25" s="5" t="s">
+        <v>118</v>
+      </c>
+      <c r="M25" s="5" t="s">
+        <v>47</v>
+      </c>
+      <c r="N25" s="5" t="s">
+        <v>30</v>
+      </c>
+      <c r="O25" s="6" t="s">
+        <v>119</v>
+      </c>
+      <c r="P25" s="6">
+        <v>240</v>
+      </c>
+      <c r="Q25" s="5"/>
+    </row>
+    <row r="26" spans="1:17">
+      <c r="A26" s="4" t="s">
+        <v>19</v>
+      </c>
+      <c r="B26" s="5" t="s">
+        <v>20</v>
+      </c>
+      <c r="C26" s="5" t="s">
+        <v>21</v>
+      </c>
+      <c r="D26" s="5" t="s">
+        <v>108</v>
+      </c>
+      <c r="E26" s="5" t="s">
+        <v>115</v>
+      </c>
+      <c r="F26" s="5" t="s">
+        <v>24</v>
+      </c>
+      <c r="G26" s="4">
+        <v>5</v>
+      </c>
+      <c r="H26" s="4">
+        <v>5</v>
+      </c>
+      <c r="I26" s="4" t="s">
+        <v>120</v>
+      </c>
+      <c r="J26" s="5" t="s">
+        <v>121</v>
+      </c>
+      <c r="K26" s="7" t="s">
+        <v>27</v>
+      </c>
+      <c r="L26" s="5" t="s">
+        <v>118</v>
+      </c>
+      <c r="M26" s="5" t="s">
+        <v>47</v>
+      </c>
+      <c r="N26" s="5" t="s">
+        <v>30</v>
+      </c>
+      <c r="O26" s="6" t="s">
+        <v>122</v>
+      </c>
+      <c r="P26" s="6">
+        <v>60</v>
+      </c>
+      <c r="Q26" s="5"/>
+    </row>
+    <row r="27" spans="1:17">
+      <c r="A27" s="4" t="s">
+        <v>19</v>
+      </c>
+      <c r="B27" s="5" t="s">
+        <v>20</v>
+      </c>
+      <c r="C27" s="5" t="s">
+        <v>21</v>
+      </c>
+      <c r="D27" s="5" t="s">
+        <v>108</v>
+      </c>
+      <c r="E27" s="5" t="s">
+        <v>123</v>
+      </c>
+      <c r="F27" s="5" t="s">
+        <v>24</v>
+      </c>
+      <c r="G27" s="4">
+        <v>2</v>
+      </c>
+      <c r="H27" s="4">
+        <v>0</v>
+      </c>
+      <c r="I27" s="4" t="s">
+        <v>124</v>
+      </c>
+      <c r="J27" s="5" t="s">
+        <v>125</v>
+      </c>
+      <c r="K27" s="7" t="s">
+        <v>27</v>
+      </c>
+      <c r="L27" s="5" t="s">
+        <v>126</v>
+      </c>
+      <c r="M27" s="5" t="s">
+        <v>36</v>
+      </c>
+      <c r="N27" s="5"/>
+      <c r="O27" s="6" t="s">
         <v>37</v>
       </c>
-      <c r="P8" s="6">
+      <c r="P27" s="6">
         <v>0</v>
       </c>
-      <c r="Q8" s="5"/>
+      <c r="Q27" s="5"/>
+    </row>
+    <row r="28" spans="1:17">
+      <c r="A28" s="4" t="s">
+        <v>19</v>
+      </c>
+      <c r="B28" s="5" t="s">
+        <v>20</v>
+      </c>
+      <c r="C28" s="5" t="s">
+        <v>21</v>
+      </c>
+      <c r="D28" s="5" t="s">
+        <v>108</v>
+      </c>
+      <c r="E28" s="5" t="s">
+        <v>127</v>
+      </c>
+      <c r="F28" s="5" t="s">
+        <v>24</v>
+      </c>
+      <c r="G28" s="4">
+        <v>2</v>
+      </c>
+      <c r="H28" s="4">
+        <v>2</v>
+      </c>
+      <c r="I28" s="4" t="s">
+        <v>25</v>
+      </c>
+      <c r="J28" s="5" t="s">
+        <v>128</v>
+      </c>
+      <c r="K28" s="7" t="s">
+        <v>27</v>
+      </c>
+      <c r="L28" s="5" t="s">
+        <v>129</v>
+      </c>
+      <c r="M28" s="5" t="s">
+        <v>47</v>
+      </c>
+      <c r="N28" s="5" t="s">
+        <v>30</v>
+      </c>
+      <c r="O28" s="6" t="s">
+        <v>130</v>
+      </c>
+      <c r="P28" s="6">
+        <v>44</v>
+      </c>
+      <c r="Q28" s="5"/>
+    </row>
+    <row r="29" spans="1:17">
+      <c r="A29" s="4" t="s">
+        <v>19</v>
+      </c>
+      <c r="B29" s="5" t="s">
+        <v>20</v>
+      </c>
+      <c r="C29" s="5" t="s">
+        <v>21</v>
+      </c>
+      <c r="D29" s="5" t="s">
+        <v>108</v>
+      </c>
+      <c r="E29" s="5" t="s">
+        <v>131</v>
+      </c>
+      <c r="F29" s="5" t="s">
+        <v>24</v>
+      </c>
+      <c r="G29" s="4">
+        <v>2</v>
+      </c>
+      <c r="H29" s="4">
+        <v>2</v>
+      </c>
+      <c r="I29" s="4" t="s">
+        <v>55</v>
+      </c>
+      <c r="J29" s="5" t="s">
+        <v>132</v>
+      </c>
+      <c r="K29" s="7" t="s">
+        <v>27</v>
+      </c>
+      <c r="L29" s="5" t="s">
+        <v>126</v>
+      </c>
+      <c r="M29" s="5" t="s">
+        <v>41</v>
+      </c>
+      <c r="N29" s="5" t="s">
+        <v>30</v>
+      </c>
+      <c r="O29" s="6" t="s">
+        <v>133</v>
+      </c>
+      <c r="P29" s="6">
+        <v>254.5</v>
+      </c>
+      <c r="Q29" s="5"/>
+    </row>
+    <row r="30" spans="1:17">
+      <c r="A30" s="4" t="s">
+        <v>19</v>
+      </c>
+      <c r="B30" s="5" t="s">
+        <v>20</v>
+      </c>
+      <c r="C30" s="5" t="s">
+        <v>21</v>
+      </c>
+      <c r="D30" s="5" t="s">
+        <v>134</v>
+      </c>
+      <c r="E30" s="5" t="s">
+        <v>135</v>
+      </c>
+      <c r="F30" s="5" t="s">
+        <v>24</v>
+      </c>
+      <c r="G30" s="4">
+        <v>5</v>
+      </c>
+      <c r="H30" s="4">
+        <v>5</v>
+      </c>
+      <c r="I30" s="4" t="s">
+        <v>33</v>
+      </c>
+      <c r="J30" s="5" t="s">
+        <v>136</v>
+      </c>
+      <c r="K30" s="7" t="s">
+        <v>27</v>
+      </c>
+      <c r="L30" s="5" t="s">
+        <v>137</v>
+      </c>
+      <c r="M30" s="5" t="s">
+        <v>41</v>
+      </c>
+      <c r="N30" s="5" t="s">
+        <v>30</v>
+      </c>
+      <c r="O30" s="6" t="s">
+        <v>138</v>
+      </c>
+      <c r="P30" s="6">
+        <v>57.25</v>
+      </c>
+      <c r="Q30" s="5"/>
+    </row>
+    <row r="31" spans="1:17">
+      <c r="A31" s="4" t="s">
+        <v>19</v>
+      </c>
+      <c r="B31" s="5" t="s">
+        <v>20</v>
+      </c>
+      <c r="C31" s="5" t="s">
+        <v>21</v>
+      </c>
+      <c r="D31" s="5" t="s">
+        <v>134</v>
+      </c>
+      <c r="E31" s="5" t="s">
+        <v>139</v>
+      </c>
+      <c r="F31" s="5" t="s">
+        <v>24</v>
+      </c>
+      <c r="G31" s="4">
+        <v>3</v>
+      </c>
+      <c r="H31" s="4">
+        <v>3</v>
+      </c>
+      <c r="I31" s="4" t="s">
+        <v>25</v>
+      </c>
+      <c r="J31" s="5" t="s">
+        <v>39</v>
+      </c>
+      <c r="K31" s="7" t="s">
+        <v>27</v>
+      </c>
+      <c r="L31" s="5" t="s">
+        <v>40</v>
+      </c>
+      <c r="M31" s="5" t="s">
+        <v>140</v>
+      </c>
+      <c r="N31" s="5" t="s">
+        <v>30</v>
+      </c>
+      <c r="O31" s="6" t="s">
+        <v>141</v>
+      </c>
+      <c r="P31" s="6">
+        <v>54</v>
+      </c>
+      <c r="Q31" s="5"/>
+    </row>
+    <row r="32" spans="1:17">
+      <c r="A32" s="4" t="s">
+        <v>19</v>
+      </c>
+      <c r="B32" s="5" t="s">
+        <v>20</v>
+      </c>
+      <c r="C32" s="5" t="s">
+        <v>21</v>
+      </c>
+      <c r="D32" s="5" t="s">
+        <v>134</v>
+      </c>
+      <c r="E32" s="5" t="s">
+        <v>142</v>
+      </c>
+      <c r="F32" s="5" t="s">
+        <v>24</v>
+      </c>
+      <c r="G32" s="4">
+        <v>2</v>
+      </c>
+      <c r="H32" s="4">
+        <v>2</v>
+      </c>
+      <c r="I32" s="4" t="s">
+        <v>55</v>
+      </c>
+      <c r="J32" s="5" t="s">
+        <v>143</v>
+      </c>
+      <c r="K32" s="7" t="s">
+        <v>27</v>
+      </c>
+      <c r="L32" s="5" t="s">
+        <v>144</v>
+      </c>
+      <c r="M32" s="5" t="s">
+        <v>52</v>
+      </c>
+      <c r="N32" s="5" t="s">
+        <v>30</v>
+      </c>
+      <c r="O32" s="6" t="s">
+        <v>145</v>
+      </c>
+      <c r="P32" s="6">
+        <v>415</v>
+      </c>
+      <c r="Q32" s="5"/>
+    </row>
+    <row r="33" spans="1:17">
+      <c r="A33" s="4" t="s">
+        <v>19</v>
+      </c>
+      <c r="B33" s="5" t="s">
+        <v>20</v>
+      </c>
+      <c r="C33" s="5" t="s">
+        <v>21</v>
+      </c>
+      <c r="D33" s="5" t="s">
+        <v>146</v>
+      </c>
+      <c r="E33" s="5" t="s">
+        <v>147</v>
+      </c>
+      <c r="F33" s="5" t="s">
+        <v>24</v>
+      </c>
+      <c r="G33" s="4">
+        <v>3</v>
+      </c>
+      <c r="H33" s="4">
+        <v>3</v>
+      </c>
+      <c r="I33" s="4" t="s">
+        <v>25</v>
+      </c>
+      <c r="J33" s="5" t="s">
+        <v>148</v>
+      </c>
+      <c r="K33" s="7" t="s">
+        <v>27</v>
+      </c>
+      <c r="L33" s="5" t="s">
+        <v>149</v>
+      </c>
+      <c r="M33" s="5" t="s">
+        <v>150</v>
+      </c>
+      <c r="N33" s="5" t="s">
+        <v>30</v>
+      </c>
+      <c r="O33" s="6" t="s">
+        <v>53</v>
+      </c>
+      <c r="P33" s="6">
+        <v>165</v>
+      </c>
+      <c r="Q33" s="5"/>
+    </row>
+    <row r="34" spans="1:17">
+      <c r="A34" s="4" t="s">
+        <v>19</v>
+      </c>
+      <c r="B34" s="5" t="s">
+        <v>20</v>
+      </c>
+      <c r="C34" s="5" t="s">
+        <v>21</v>
+      </c>
+      <c r="D34" s="5" t="s">
+        <v>146</v>
+      </c>
+      <c r="E34" s="5" t="s">
+        <v>151</v>
+      </c>
+      <c r="F34" s="5" t="s">
+        <v>24</v>
+      </c>
+      <c r="G34" s="4">
+        <v>1</v>
+      </c>
+      <c r="H34" s="4">
+        <v>1</v>
+      </c>
+      <c r="I34" s="4" t="s">
+        <v>25</v>
+      </c>
+      <c r="J34" s="5" t="s">
+        <v>152</v>
+      </c>
+      <c r="K34" s="7" t="s">
+        <v>27</v>
+      </c>
+      <c r="L34" s="5" t="s">
+        <v>153</v>
+      </c>
+      <c r="M34" s="5" t="s">
+        <v>154</v>
+      </c>
+      <c r="N34" s="5" t="s">
+        <v>30</v>
+      </c>
+      <c r="O34" s="6" t="s">
+        <v>155</v>
+      </c>
+      <c r="P34" s="6">
+        <v>70</v>
+      </c>
+      <c r="Q34" s="5"/>
+    </row>
+    <row r="35" spans="1:17">
+      <c r="A35" s="4" t="s">
+        <v>19</v>
+      </c>
+      <c r="B35" s="5" t="s">
+        <v>20</v>
+      </c>
+      <c r="C35" s="5" t="s">
+        <v>21</v>
+      </c>
+      <c r="D35" s="5" t="s">
+        <v>146</v>
+      </c>
+      <c r="E35" s="5" t="s">
+        <v>156</v>
+      </c>
+      <c r="F35" s="5" t="s">
+        <v>24</v>
+      </c>
+      <c r="G35" s="4">
+        <v>4</v>
+      </c>
+      <c r="H35" s="4">
+        <v>4</v>
+      </c>
+      <c r="I35" s="4" t="s">
+        <v>157</v>
+      </c>
+      <c r="J35" s="5" t="s">
+        <v>158</v>
+      </c>
+      <c r="K35" s="7" t="s">
+        <v>27</v>
+      </c>
+      <c r="L35" s="5" t="s">
+        <v>159</v>
+      </c>
+      <c r="M35" s="5" t="s">
+        <v>160</v>
+      </c>
+      <c r="N35" s="5" t="s">
+        <v>30</v>
+      </c>
+      <c r="O35" s="6" t="s">
+        <v>161</v>
+      </c>
+      <c r="P35" s="6">
+        <v>40</v>
+      </c>
+      <c r="Q35" s="5"/>
+    </row>
+    <row r="36" spans="1:17">
+      <c r="A36" s="4" t="s">
+        <v>19</v>
+      </c>
+      <c r="B36" s="5" t="s">
+        <v>20</v>
+      </c>
+      <c r="C36" s="5" t="s">
+        <v>21</v>
+      </c>
+      <c r="D36" s="5" t="s">
+        <v>146</v>
+      </c>
+      <c r="E36" s="5" t="s">
+        <v>162</v>
+      </c>
+      <c r="F36" s="5" t="s">
+        <v>24</v>
+      </c>
+      <c r="G36" s="4">
+        <v>1</v>
+      </c>
+      <c r="H36" s="4">
+        <v>1</v>
+      </c>
+      <c r="I36" s="4" t="s">
+        <v>163</v>
+      </c>
+      <c r="J36" s="5" t="s">
+        <v>164</v>
+      </c>
+      <c r="K36" s="7" t="s">
+        <v>27</v>
+      </c>
+      <c r="L36" s="5" t="s">
+        <v>165</v>
+      </c>
+      <c r="M36" s="5" t="s">
+        <v>29</v>
+      </c>
+      <c r="N36" s="5" t="s">
+        <v>30</v>
+      </c>
+      <c r="O36" s="6" t="s">
+        <v>166</v>
+      </c>
+      <c r="P36" s="6">
+        <v>45</v>
+      </c>
+      <c r="Q36" s="5"/>
+    </row>
+    <row r="37" spans="1:17">
+      <c r="A37" s="4" t="s">
+        <v>19</v>
+      </c>
+      <c r="B37" s="5" t="s">
+        <v>20</v>
+      </c>
+      <c r="C37" s="5" t="s">
+        <v>21</v>
+      </c>
+      <c r="D37" s="5" t="s">
+        <v>146</v>
+      </c>
+      <c r="E37" s="5" t="s">
+        <v>167</v>
+      </c>
+      <c r="F37" s="5" t="s">
+        <v>24</v>
+      </c>
+      <c r="G37" s="4">
+        <v>8</v>
+      </c>
+      <c r="H37" s="4">
+        <v>8</v>
+      </c>
+      <c r="I37" s="4" t="s">
+        <v>168</v>
+      </c>
+      <c r="J37" s="5" t="s">
+        <v>169</v>
+      </c>
+      <c r="K37" s="7" t="s">
+        <v>27</v>
+      </c>
+      <c r="L37" s="5" t="s">
+        <v>170</v>
+      </c>
+      <c r="M37" s="5" t="s">
+        <v>52</v>
+      </c>
+      <c r="N37" s="5" t="s">
+        <v>30</v>
+      </c>
+      <c r="O37" s="6" t="s">
+        <v>171</v>
+      </c>
+      <c r="P37" s="6">
+        <v>248</v>
+      </c>
+      <c r="Q37" s="5"/>
+    </row>
+    <row r="38" spans="1:17">
+      <c r="A38" s="4" t="s">
+        <v>19</v>
+      </c>
+      <c r="B38" s="5" t="s">
+        <v>20</v>
+      </c>
+      <c r="C38" s="5" t="s">
+        <v>21</v>
+      </c>
+      <c r="D38" s="5" t="s">
+        <v>172</v>
+      </c>
+      <c r="E38" s="5" t="s">
+        <v>173</v>
+      </c>
+      <c r="F38" s="5" t="s">
+        <v>24</v>
+      </c>
+      <c r="G38" s="4">
+        <v>20</v>
+      </c>
+      <c r="H38" s="4">
+        <v>20</v>
+      </c>
+      <c r="I38" s="4" t="s">
+        <v>55</v>
+      </c>
+      <c r="J38" s="5" t="s">
+        <v>174</v>
+      </c>
+      <c r="K38" s="7" t="s">
+        <v>27</v>
+      </c>
+      <c r="L38" s="5" t="s">
+        <v>175</v>
+      </c>
+      <c r="M38" s="5" t="s">
+        <v>69</v>
+      </c>
+      <c r="N38" s="5" t="s">
+        <v>70</v>
+      </c>
+      <c r="O38" s="6" t="s">
+        <v>176</v>
+      </c>
+      <c r="P38" s="6">
+        <v>1500</v>
+      </c>
+      <c r="Q38" s="5"/>
+    </row>
+    <row r="39" spans="1:17">
+      <c r="A39" s="4" t="s">
+        <v>19</v>
+      </c>
+      <c r="B39" s="5" t="s">
+        <v>20</v>
+      </c>
+      <c r="C39" s="5" t="s">
+        <v>21</v>
+      </c>
+      <c r="D39" s="5" t="s">
+        <v>172</v>
+      </c>
+      <c r="E39" s="5" t="s">
+        <v>173</v>
+      </c>
+      <c r="F39" s="5" t="s">
+        <v>24</v>
+      </c>
+      <c r="G39" s="4">
+        <v>20</v>
+      </c>
+      <c r="H39" s="4">
+        <v>20</v>
+      </c>
+      <c r="I39" s="4" t="s">
+        <v>55</v>
+      </c>
+      <c r="J39" s="5" t="s">
+        <v>177</v>
+      </c>
+      <c r="K39" s="7" t="s">
+        <v>27</v>
+      </c>
+      <c r="L39" s="5" t="s">
+        <v>175</v>
+      </c>
+      <c r="M39" s="5" t="s">
+        <v>69</v>
+      </c>
+      <c r="N39" s="5" t="s">
+        <v>70</v>
+      </c>
+      <c r="O39" s="6" t="s">
+        <v>178</v>
+      </c>
+      <c r="P39" s="6">
+        <v>3600</v>
+      </c>
+      <c r="Q39" s="5"/>
+    </row>
+    <row r="40" spans="1:17">
+      <c r="A40" s="4" t="s">
+        <v>19</v>
+      </c>
+      <c r="B40" s="5" t="s">
+        <v>20</v>
+      </c>
+      <c r="C40" s="5" t="s">
+        <v>21</v>
+      </c>
+      <c r="D40" s="5" t="s">
+        <v>179</v>
+      </c>
+      <c r="E40" s="5" t="s">
+        <v>180</v>
+      </c>
+      <c r="F40" s="5" t="s">
+        <v>24</v>
+      </c>
+      <c r="G40" s="4">
+        <v>1</v>
+      </c>
+      <c r="H40" s="4">
+        <v>1</v>
+      </c>
+      <c r="I40" s="4" t="s">
+        <v>181</v>
+      </c>
+      <c r="J40" s="5" t="s">
+        <v>182</v>
+      </c>
+      <c r="K40" s="7" t="s">
+        <v>27</v>
+      </c>
+      <c r="L40" s="5" t="s">
+        <v>183</v>
+      </c>
+      <c r="M40" s="5" t="s">
+        <v>100</v>
+      </c>
+      <c r="N40" s="5" t="s">
+        <v>101</v>
+      </c>
+      <c r="O40" s="6" t="s">
+        <v>184</v>
+      </c>
+      <c r="P40" s="6">
+        <v>72</v>
+      </c>
+      <c r="Q40" s="5"/>
+    </row>
+    <row r="41" spans="1:17">
+      <c r="A41" s="4" t="s">
+        <v>19</v>
+      </c>
+      <c r="B41" s="5" t="s">
+        <v>20</v>
+      </c>
+      <c r="C41" s="5" t="s">
+        <v>21</v>
+      </c>
+      <c r="D41" s="5" t="s">
+        <v>185</v>
+      </c>
+      <c r="E41" s="5" t="s">
+        <v>186</v>
+      </c>
+      <c r="F41" s="5" t="s">
+        <v>24</v>
+      </c>
+      <c r="G41" s="4">
+        <v>3</v>
+      </c>
+      <c r="H41" s="4">
+        <v>3</v>
+      </c>
+      <c r="I41" s="4" t="s">
+        <v>110</v>
+      </c>
+      <c r="J41" s="5" t="s">
+        <v>187</v>
+      </c>
+      <c r="K41" s="7" t="s">
+        <v>27</v>
+      </c>
+      <c r="L41" s="5" t="s">
+        <v>188</v>
+      </c>
+      <c r="M41" s="5" t="s">
+        <v>189</v>
+      </c>
+      <c r="N41" s="5" t="s">
+        <v>30</v>
+      </c>
+      <c r="O41" s="6" t="s">
+        <v>122</v>
+      </c>
+      <c r="P41" s="6">
+        <v>36</v>
+      </c>
+      <c r="Q41" s="5"/>
     </row>
   </sheetData>
   <sheetProtection sheet="false" objects="false" scenarios="false" formatCells="false" formatColumns="false" formatRows="false" insertColumns="false" insertRows="false" insertHyperlinks="false" deleteColumns="false" deleteRows="false" selectLockedCells="false" sort="false" autoFilter="false" pivotTables="false" selectUnlockedCells="false"/>

</xml_diff>